<commit_message>
fix sci extension in xls
</commit_message>
<xml_diff>
--- a/csv/xls.xlsx
+++ b/csv/xls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vunl-my.sharepoint.com/personal/lena_reimann_vu_nl/Documents/Documents/GitHub/climate-risk-stac/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{D4CAE234-722A-4C5E-A7B5-791925D7A1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E7E571D-0780-4A5E-BBA9-B1A0E29DB48E}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{D4CAE234-722A-4C5E-A7B5-791925D7A1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEE4C983-93C6-4CBF-9B0E-D57FCE944FD3}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-3180" windowWidth="25180" windowHeight="16140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -208,7 +208,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5583" uniqueCount="1192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5583" uniqueCount="1193">
   <si>
     <t xml:space="preserve">Instructions: How to fill in the data sheet? </t>
   </si>
@@ -4105,6 +4105,9 @@
   </si>
   <si>
     <t>https://doi.org/10.1016/j.ejrh.2019.100593</t>
+  </si>
+  <si>
+    <t>10.7910/DVN/PRFF8V</t>
   </si>
 </sst>
 </file>
@@ -14613,8 +14616,8 @@
   </sheetPr>
   <dimension ref="A1:AI201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AA110" sqref="AA110"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15109,10 +15112,10 @@
         <v>513</v>
       </c>
       <c r="AB5" s="39" t="s">
-        <v>514</v>
+        <v>1192</v>
       </c>
       <c r="AC5" s="32" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="AD5" s="32"/>
       <c r="AE5" s="32"/>
@@ -29009,7 +29012,7 @@
     <hyperlink ref="AB80" r:id="rId72" xr:uid="{9857F2DA-7A2F-41F7-89A8-C3C9A24B4CB1}"/>
     <hyperlink ref="AG80" r:id="rId73" xr:uid="{E1AC70FF-C2FE-475A-B568-24ED10875CF7}"/>
     <hyperlink ref="AA5" r:id="rId74" xr:uid="{B4903B9B-343D-4C94-90CF-B09CAFB06F57}"/>
-    <hyperlink ref="AB5" r:id="rId75" xr:uid="{5AE1B450-62FE-4A87-9230-137A08A21D92}"/>
+    <hyperlink ref="AB5" r:id="rId75" display="https://doi.org/10.7910/DVN/PRFF8V" xr:uid="{5AE1B450-62FE-4A87-9230-137A08A21D92}"/>
     <hyperlink ref="AG5" r:id="rId76" xr:uid="{4EFBE8AC-E871-43EF-BD8D-79B9874C3D70}"/>
     <hyperlink ref="AA28" r:id="rId77" xr:uid="{8497F84F-6543-42B9-9361-58EF7A4BD28B}"/>
     <hyperlink ref="AB28" r:id="rId78" xr:uid="{5416741B-C7A3-400B-8D3E-5C3654BAF644}"/>

</xml_diff>

<commit_message>
sci ext fix v2
</commit_message>
<xml_diff>
--- a/csv/xls.xlsx
+++ b/csv/xls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vunl-my.sharepoint.com/personal/lena_reimann_vu_nl/Documents/Documents/GitHub/climate-risk-stac/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{D4CAE234-722A-4C5E-A7B5-791925D7A1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEE4C983-93C6-4CBF-9B0E-D57FCE944FD3}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{D4CAE234-722A-4C5E-A7B5-791925D7A1A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B48B35DF-8174-4148-84CE-9D08FBD30479}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-3180" windowWidth="25180" windowHeight="16140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-3180" windowWidth="25180" windowHeight="16140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="4" r:id="rId1"/>
@@ -4104,10 +4104,10 @@
     <t>https://gwis-reports.s3-eu-west-1.amazonaws.com/WFRA/var-vuln-econ_unit-dimensionless.zip</t>
   </si>
   <si>
-    <t>https://doi.org/10.1016/j.ejrh.2019.100593</t>
-  </si>
-  <si>
     <t>10.7910/DVN/PRFF8V</t>
+  </si>
+  <si>
+    <t>10.1016/j.ejrh.2019.100593</t>
   </si>
 </sst>
 </file>
@@ -4811,7 +4811,7 @@
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4900,6 +4900,7 @@
     <xf numFmtId="0" fontId="21" fillId="36" borderId="0" xfId="42" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="42" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="23" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" xfId="42" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -7138,8 +7139,8 @@
   </sheetPr>
   <dimension ref="A1:AI208"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7540,8 +7541,8 @@
       <c r="AA4" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="AB4" s="48" t="s">
-        <v>1191</v>
+      <c r="AB4" s="72" t="s">
+        <v>1192</v>
       </c>
       <c r="AC4" t="s">
         <v>91</v>
@@ -7633,7 +7634,7 @@
       <c r="AA5" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="AB5" s="10" t="s">
+      <c r="AB5" s="72" t="s">
         <v>107</v>
       </c>
       <c r="AC5" s="9" t="s">
@@ -14511,7 +14512,7 @@
     <hyperlink ref="AB6" r:id="rId37" xr:uid="{EABAB9C8-0B91-4A98-9C82-4A419970BA9A}"/>
     <hyperlink ref="AB7" r:id="rId38" xr:uid="{9F0561D3-7E24-42D9-8C4E-CD5C3B88764D}"/>
     <hyperlink ref="AB8" r:id="rId39" xr:uid="{CDC3BCD6-225C-43B9-BCCA-418F09827512}"/>
-    <hyperlink ref="AB4" r:id="rId40" xr:uid="{3E877577-8842-4798-99D6-DF26D7A6D6C9}"/>
+    <hyperlink ref="AB4" r:id="rId40" display="https://doi.org/10.1016/j.ejrh.2019.100593" xr:uid="{3E877577-8842-4798-99D6-DF26D7A6D6C9}"/>
     <hyperlink ref="AA44" r:id="rId41" location="!/dataset/sis-tourism-fire-danger-indicators?tab=overview" xr:uid="{96CB8A9E-64DC-40E3-A5CD-91038727F9C9}"/>
     <hyperlink ref="AG33" r:id="rId42" display="https://cidportal.jrc.ec.europa.eu/ftp/jrc-opendata/FLOODS/GlobalMaps/floodMapGL_rp10y.zip;https://cidportal.jrc.ec.europa.eu/ftp/jrc-opendata/FLOODS/GlobalMaps/floodMapGL_rp20y.zip;https://cidportal.jrc.ec.europa.eu/ftp/jrc-opendata/FLOODS/GlobalMaps/floodMapGL_rp50y.zip;https://cidportal.jrc.ec.europa.eu/ftp/jrc-opendata/FLOODS/GlobalMaps/floodMapGL_rp100y.zip;https://cidportal.jrc.ec.europa.eu/ftp/jrc-opendata/FLOODS/GlobalMaps/floodMapGL_rp200y.zip;https://cidportal.jrc.ec.europa.eu/ftp/jrc-opendata/FLOODS/GlobalMaps/floodMapGL_rp500y.zip" xr:uid="{17E6576C-18D2-434D-8A6E-F0C2BFE1894E}"/>
     <hyperlink ref="AA45" r:id="rId43" location="!/dataset/10.24381/cds.0e89c522?tab=overview" xr:uid="{0CF63EAD-38AE-4DC7-971F-BFBAE804BE2F}"/>
@@ -14616,8 +14617,8 @@
   </sheetPr>
   <dimension ref="A1:AI201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AC5" sqref="AC5"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AB5" sqref="AB5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15112,7 +15113,7 @@
         <v>513</v>
       </c>
       <c r="AB5" s="39" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="AC5" s="32" t="s">
         <v>91</v>

</xml_diff>